<commit_message>
semi-stable version with handling of network speeds
</commit_message>
<xml_diff>
--- a/data/datapoint_mapping.xlsx
+++ b/data/datapoint_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miloe\Desktop\etf_web_scrape\etf_web_scrape\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FA260C-8A02-4375-B666-BB9F19B28969}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E1C42C-FDF4-47F4-A5DB-1E3FEFAA7D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30870" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{A2580E61-6539-4FBC-BE58-C02B7719626C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2580E61-6539-4FBC-BE58-C02B7719626C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>website</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>fund_aum_asof</t>
+  </si>
+  <si>
+    <t>investment_objective</t>
+  </si>
+  <si>
+    <t>fund-objective-card-content</t>
   </si>
 </sst>
 </file>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB954058-E30C-4B39-981A-19498E608132}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +843,17 @@
         <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -866,8 +883,9 @@
     <hyperlink ref="C23" r:id="rId22" xr:uid="{256C8D72-7943-4FA2-BA62-73747D637628}"/>
     <hyperlink ref="C24" r:id="rId23" xr:uid="{EA9684F3-3E87-454F-BD90-E4924A098962}"/>
     <hyperlink ref="C25" r:id="rId24" xr:uid="{8354EAA5-962F-4A01-95B6-E6507AD30F07}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{9D7232FD-C3A6-41F1-BF56-B4207C43019F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
addition of get ISINs method for JPM ETFs
</commit_message>
<xml_diff>
--- a/data/datapoint_mapping.xlsx
+++ b/data/datapoint_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miloe\Desktop\etf_web_scrape\etf_web_scrape\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E1C42C-FDF4-47F4-A5DB-1E3FEFAA7D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59341EA2-599E-4BF8-9BFF-BA71D1687768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2580E61-6539-4FBC-BE58-C02B7719626C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>website</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>fund-objective-card-content</t>
+  </si>
+  <si>
+    <t>fund_name</t>
+  </si>
+  <si>
+    <t>summary-header-fund-name</t>
+  </si>
+  <si>
+    <t>shareclass_name</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -558,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB954058-E30C-4B39-981A-19498E608132}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +866,28 @@
         <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -884,8 +918,10 @@
     <hyperlink ref="C24" r:id="rId23" xr:uid="{EA9684F3-3E87-454F-BD90-E4924A098962}"/>
     <hyperlink ref="C25" r:id="rId24" xr:uid="{8354EAA5-962F-4A01-95B6-E6507AD30F07}"/>
     <hyperlink ref="C26" r:id="rId25" xr:uid="{9D7232FD-C3A6-41F1-BF56-B4207C43019F}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{E3856B45-78AB-4586-8854-2BB9CEDCB954}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{FF9B8C62-9153-4C1D-9B57-EAD2FE1FB695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
addition of dist/acc logic
</commit_message>
<xml_diff>
--- a/data/datapoint_mapping.xlsx
+++ b/data/datapoint_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miloe\Desktop\etf_web_scrape\etf_web_scrape\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59341EA2-599E-4BF8-9BFF-BA71D1687768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF7E6A7-0B5F-49C3-A6AA-1345508B16A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2580E61-6539-4FBC-BE58-C02B7719626C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>website</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>shareclass_dist_status</t>
+  </si>
+  <si>
+    <t>shareclass_assets</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB954058-E30C-4B39-981A-19498E608132}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,6 +894,28 @@
         <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -920,8 +948,10 @@
     <hyperlink ref="C26" r:id="rId25" xr:uid="{9D7232FD-C3A6-41F1-BF56-B4207C43019F}"/>
     <hyperlink ref="C27" r:id="rId26" xr:uid="{E3856B45-78AB-4586-8854-2BB9CEDCB954}"/>
     <hyperlink ref="C28" r:id="rId27" xr:uid="{FF9B8C62-9153-4C1D-9B57-EAD2FE1FB695}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{4F262CCB-A6D7-48A7-A290-EE0F551A413A}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{D69E8856-CF66-4E2E-B3B3-1F2162EFB8AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId28"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>